<commit_message>
[MOSIP-21520] updated mosip-data for hindi,kannada, and tamil language
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -297,8 +297,8 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated the loc_hierarchy_list file
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E03E66-120C-4100-A5A3-D8028384D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B9BDBC-2361-4987-B39D-9282B411DD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$19</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>lang_code</t>
   </si>
@@ -57,10 +57,49 @@
     <t>Postal Code</t>
   </si>
   <si>
-    <t>World</t>
-  </si>
-  <si>
-    <t>Municipality</t>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>ara</t>
+  </si>
+  <si>
+    <t>دولة</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>Pays</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>المناطق</t>
+  </si>
+  <si>
+    <t>Région</t>
+  </si>
+  <si>
+    <t>المحافظة</t>
+  </si>
+  <si>
+    <t>مدينة</t>
+  </si>
+  <si>
+    <t>Ville</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>منطقة</t>
+  </si>
+  <si>
+    <t>رمز بريدي</t>
+  </si>
+  <si>
+    <t>code postal</t>
   </si>
 </sst>
 </file>
@@ -129,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -139,6 +178,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,94 +523,262 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="b">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="B18">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D19" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Updated the loc_hierarchy_list file with only ENG as lang
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B9BDBC-2361-4987-B39D-9282B411DD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F1AD4-C1F1-4312-A2E5-51812400AB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>lang_code</t>
   </si>
@@ -60,46 +60,10 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>دولة</t>
-  </si>
-  <si>
-    <t>fra</t>
-  </si>
-  <si>
-    <t>Pays</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>المناطق</t>
-  </si>
-  <si>
-    <t>Région</t>
-  </si>
-  <si>
-    <t>المحافظة</t>
-  </si>
-  <si>
-    <t>مدينة</t>
-  </si>
-  <si>
-    <t>Ville</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>منطقة</t>
-  </si>
-  <si>
-    <t>رمز بريدي</t>
-  </si>
-  <si>
-    <t>code postal</t>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Municipality</t>
   </si>
 </sst>
 </file>
@@ -118,7 +82,7 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="6"/>
@@ -496,7 +460,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,8 +493,8 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
@@ -539,13 +503,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
@@ -554,13 +518,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
@@ -572,10 +536,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -584,13 +548,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -599,13 +563,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -613,172 +577,73 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D19" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
MOSIP-29415 Fixed Foreign key constraint issue for Location code cardigo portal in spanish language. (#266)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17190E33-073C-4773-B1C5-40B8570035F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E270E-8711-441F-A8F3-D7BA84F14BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>Zona</t>
   </si>
   <si>
-    <t>Código Postal</t>
+    <t xml:space="preserve"> Código Postal</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1175,7 @@
       <c r="B43">
         <v>5</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">

</xml_diff>